<commit_message>
Database Demo Data Updated!
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66694E0F-BC1D-4F87-893F-C8637ABBDF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57BB4F3-104B-4296-A317-FA2D71E410F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="119">
   <si>
     <t>🔒 PROTECTED: Description formulas &amp; formatting are locked. DELETE key is safe to use!</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Tasks for everyone with option to assign to employees if required</t>
   </si>
   <si>
     <t xml:space="preserve">  📋 EXCEL TASK CALENDAR - USER GUIDE</t>
@@ -656,16 +659,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -686,6 +679,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,7 +1081,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1093,26 +1096,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" ht="24.95" customHeight="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
@@ -18267,14 +18270,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="42.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -18289,7 +18292,9 @@
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
@@ -22286,9 +22291,9 @@
       <c r="B1000" s="10"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="X6RMM6NRWGmtulYkRzY6vZ0Sk2OAu0h8NsDgNeCevuLqT8+AEYvtKNxTjuSQpNtULe6Qo5LuhkjIhLR8lskQSQ==" saltValue="Hd3Zo+wZaCFJr9MZVa4wCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oeZaNLQ9AWY6Msdt4n3voFUT6Smc/SkknCdpk3p4g3Vj1eJfETeQgVZHm1ifcXnKhzJysLwLoZvY7cC9i2cTCQ==" saltValue="nNSc2/Vv3X3zqFXGp5/GPg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="A2:B1000" name="Range1"/>
+    <protectedRange sqref="A3:B1000" name="Range1"/>
   </protectedRanges>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -22298,7 +22303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
@@ -22309,7 +22314,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22317,7 +22322,7 @@
     </row>
     <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22325,17 +22330,17 @@
     </row>
     <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
-        <v>29</v>
+      <c r="A7" s="23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22343,17 +22348,17 @@
     </row>
     <row r="9" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22361,35 +22366,35 @@
     </row>
     <row r="13" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="27" t="s">
-        <v>35</v>
+      <c r="A16" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22397,17 +22402,17 @@
     </row>
     <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="27" t="s">
-        <v>41</v>
+      <c r="A23" s="23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22415,17 +22420,17 @@
     </row>
     <row r="25" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22433,17 +22438,17 @@
     </row>
     <row r="29" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22451,81 +22456,81 @@
     </row>
     <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="28" t="s">
-        <v>47</v>
+      <c r="A34" s="24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8"/>
     </row>
     <row r="36" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="28" t="s">
-        <v>48</v>
+      <c r="A36" s="24" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="7"/>
     </row>
     <row r="41" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="29" t="s">
-        <v>52</v>
+      <c r="A41" s="25" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="8"/>
     </row>
     <row r="46" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="28" t="s">
-        <v>56</v>
+      <c r="A46" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="32" t="s">
-        <v>59</v>
+      <c r="A49" s="28" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22533,81 +22538,81 @@
     </row>
     <row r="51" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="28" t="s">
-        <v>60</v>
+      <c r="A52" s="24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A54" s="31" t="s">
-        <v>61</v>
+      <c r="A54" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="6"/>
     </row>
     <row r="60" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="31" t="s">
-        <v>66</v>
+      <c r="A60" s="27" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="7"/>
     </row>
     <row r="65" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="30" t="s">
-        <v>70</v>
+      <c r="A65" s="26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22615,12 +22620,12 @@
     </row>
     <row r="69" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A70" s="29" t="s">
-        <v>73</v>
+      <c r="A70" s="25" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22628,95 +22633,95 @@
     </row>
     <row r="72" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A76" s="27" t="s">
-        <v>78</v>
+      <c r="A76" s="23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A81" s="8"/>
     </row>
     <row r="82" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A82" s="28" t="s">
-        <v>83</v>
+      <c r="A82" s="24" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A85" s="27" t="s">
-        <v>86</v>
+      <c r="A85" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A86" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22724,156 +22729,156 @@
     </row>
     <row r="92" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:1"/>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.75">
-      <c r="A100" s="26" t="s">
-        <v>98</v>
+      <c r="A100" s="22" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:1"/>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:1"/>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.75">
-      <c r="A108" s="26" t="s">
-        <v>103</v>
+      <c r="A108" s="22" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:1"/>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:1"/>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:1"/>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:1"/>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:1"/>
     <row r="128" spans="1:1"/>
     <row r="129" spans="1:1" ht="21">
-      <c r="A129" s="33" t="s">
-        <v>117</v>
+      <c r="A129" s="29" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="130" spans="1:1"/>

</xml_diff>

<commit_message>
Added README and updated Database.xlsx
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57BB4F3-104B-4296-A317-FA2D71E410F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2D8ECE9-5E4B-4626-AFE2-055AD32052A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
     <t xml:space="preserve">  4. Upload to HTML app and start tracking!</t>
   </si>
   <si>
-    <t>Need help or have suggestions or feedback? find me on Slack: @Mohajiho</t>
+    <t>Need help or have suggestions or feedback? find me online : @Mohajiho</t>
   </si>
 </sst>
 </file>
@@ -13153,7 +13153,7 @@
       <c r="G1000" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="x/2QBb2/7D8Pb+tP2SPP9q66T/bMKa+UQ/Vsy65zjYFTTa+OM4HLgihJqU0ATbYTMGOtFQ4VjMIYX3fhdG80iQ==" saltValue="KBcrfrZgXcqs0GzNJQGerQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5rxh55fVoXCzuV0cdVDbe5efwOUWY6x0eOX/rLtHoD9/+gZg/qgSXt1yO5r922SqJgNAtm7VxXTUTCpUPIDxwA==" saltValue="A8kEMkAGv//0tRffib0Pww==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="A4:C1000" name="Range1"/>
     <protectedRange sqref="E4:G1000" name="Range2"/>
@@ -18255,7 +18255,7 @@
       <c r="C1000" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="USkqHVmuPOxkb5j7sbDlqRkRBp0ZIXSJa7+uVjeyiNg0g5KHPfG1CZZCLX0z4rgT9W0bOK7aprUE1bCvSCIruQ==" saltValue="1Gd4Pp0liIqtrEs2vCYIxA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DwofTSRJFJWXPzo5wZi0qUwKE63utsIvtBMXGO1nHV1Zw84CimHut/wOisXRcqk8dVosAY9gKjJAkP88qTe/0A==" saltValue="qe80E5YyaCdu/pwtpTtFTQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="A2:B1000" name="Range1"/>
   </protectedRanges>
@@ -18270,7 +18270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -22291,7 +22291,7 @@
       <c r="B1000" s="10"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oeZaNLQ9AWY6Msdt4n3voFUT6Smc/SkknCdpk3p4g3Vj1eJfETeQgVZHm1ifcXnKhzJysLwLoZvY7cC9i2cTCQ==" saltValue="nNSc2/Vv3X3zqFXGp5/GPg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="imB4n7dZbM8Htt7SunfEhhn28zStj1h5P3KLtK1mJXDiJ+q+g9vSLNMB4NK6JUTjIJ0qBQgRksjsnVTpI1LjZQ==" saltValue="4Eo3w2yvnFAaIyqx2p8hLg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="A3:B1000" name="Range1"/>
   </protectedRanges>
@@ -22303,8 +22303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A130"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -22883,7 +22883,7 @@
     </row>
     <row r="130" spans="1:1"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/4rDZa6nW8I4wVlmrOoaUIiuDmpn1Yem/ne/pwLyzebxyta41FOVT6AyElDv20wNFbvismwIeNrYqTm7yezSqw==" saltValue="U8UGqJ1bNIwQ0E7lequ/cA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="LWO/cjxw+wC0z0l6cSzitWfBo56wDZNC9OKHAVddU0mURnWpF02I5IKHA3E3rc05plbPOuPJaipVorT3JwLmaw==" saltValue="i/hyG32DxJiS60ETH1IHKg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All-Day tasks added to TaskManager.html!
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2D8ECE9-5E4B-4626-AFE2-055AD32052A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63105AD9-3D99-4D23-ABFF-1B7B8A7E4FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
   <si>
     <t>🔒 PROTECTED: Description formulas &amp; formatting are locked. DELETE key is safe to use!</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Replenish</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
   <si>
     <t>TaskName</t>
@@ -1080,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1237,76 +1240,138 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="20">
+        <v>45981</v>
+      </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="3" t="str">
         <f>IF(C8="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C8,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
-        <v/>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
+        <v>Description is Optional</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="20">
+        <v>45981</v>
+      </c>
       <c r="B9" s="21"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" s="3" t="str">
         <f>IF(C9="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C9,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20"/>
+      <c r="A10" s="20">
+        <v>45981</v>
+      </c>
       <c r="B10" s="21"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="3" t="str">
         <f>IF(C10="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C10,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
-        <v/>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
+        <v>Entire Store</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="20">
+        <v>45981</v>
+      </c>
+      <c r="B11" s="21">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D11" s="3" t="str">
         <f>IF(C11="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C11,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="12"/>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="20">
+        <v>45981</v>
+      </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D12" s="3" t="str">
         <f>IF(C12="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C12,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="12"/>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20"/>
+      <c r="A13" s="20">
+        <v>45981</v>
+      </c>
       <c r="B13" s="21"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D13" s="3" t="str">
         <f>IF(C13="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C13,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
-        <v/>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="12"/>
+        <v>VMI Only</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="20"/>
@@ -13238,7 +13303,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>5</v>
@@ -13250,7 +13315,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="14"/>
     </row>
@@ -13266,7 +13331,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="14"/>
     </row>
@@ -13275,7 +13340,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -18282,10 +18347,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18293,7 +18358,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -22303,7 +22368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
@@ -22314,7 +22379,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22322,7 +22387,7 @@
     </row>
     <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22330,17 +22395,17 @@
     </row>
     <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22348,17 +22413,17 @@
     </row>
     <row r="9" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22366,12 +22431,12 @@
     </row>
     <row r="13" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22379,22 +22444,22 @@
     </row>
     <row r="16" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22402,17 +22467,17 @@
     </row>
     <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22420,17 +22485,17 @@
     </row>
     <row r="25" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22438,17 +22503,17 @@
     </row>
     <row r="29" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22456,12 +22521,12 @@
     </row>
     <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22469,22 +22534,22 @@
     </row>
     <row r="36" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22492,22 +22557,22 @@
     </row>
     <row r="41" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22515,22 +22580,22 @@
     </row>
     <row r="46" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22538,12 +22603,12 @@
     </row>
     <row r="51" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22551,27 +22616,27 @@
     </row>
     <row r="54" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22579,22 +22644,22 @@
     </row>
     <row r="60" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22602,17 +22667,17 @@
     </row>
     <row r="65" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22620,12 +22685,12 @@
     </row>
     <row r="69" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22633,47 +22698,47 @@
     </row>
     <row r="72" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A76" s="23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22681,47 +22746,47 @@
     </row>
     <row r="82" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A82" s="24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A85" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A86" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22729,156 +22794,156 @@
     </row>
     <row r="92" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:1"/>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.75">
       <c r="A100" s="22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:1"/>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1"/>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.75">
       <c r="A108" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:1"/>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:1"/>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118" spans="1:1"/>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:1"/>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="127" spans="1:1"/>
     <row r="128" spans="1:1"/>
     <row r="129" spans="1:1" ht="21">
       <c r="A129" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="130" spans="1:1"/>

</xml_diff>

<commit_message>
Updated DB and README.md with latest instructions!
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D88C84C9-9191-49AC-BF5B-D8D42B9DDBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C5CA640-EA9F-4075-88BD-D5DDEC2CAD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="131">
   <si>
     <t>🔒 PROTECTED: Description formulas &amp; formatting are locked. DELETE key is safe to use!</t>
   </si>
@@ -77,16 +77,13 @@
     <t>Everyone</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Go Find</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Gap Scan</t>
+    <t>Test</t>
   </si>
   <si>
     <t>Low</t>
@@ -98,7 +95,7 @@
     <t>Replenish</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Gap Scan</t>
   </si>
   <si>
     <t>TaskName</t>
@@ -123,6 +120,135 @@
   </si>
   <si>
     <t xml:space="preserve">  📋 EXCEL TASK CALENDAR - USER GUIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ⚠️ IMPORTANT TO KNOW:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - ✅ Has date + Has time = Timed task for that date</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">  - ✅ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>No</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> date  + Has time = Everyday timed task</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">  - ✅ Has date + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>No</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> time  = All-day task for that date</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">  - ✅ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>No</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> date  + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>No</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF495057"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> time  = All-day task for every date/day if available</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  ✅ Proper handling of defaults in Database import in case of missing parameters:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - ✅ No Date: "Everyday"    (Refer to "⚠️ IMPORTANT TO KNOW" section for complete handling of Date and Time scenarios)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - ✅ No Time: "All Day"    (Refer to "⚠️ IMPORTANT TO KNOW" section for complete handling of Date and Time scenarios)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - ✅ No Priority: "Low"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - ✅ No Assignee: "Everyone"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - ✅ No Status: "Pending"</t>
   </si>
   <si>
     <t xml:space="preserve">  ✅ REQUIRED FORMAT:</t>
@@ -386,19 +512,22 @@
     <t xml:space="preserve">  Quick Start:</t>
   </si>
   <si>
-    <t xml:space="preserve">  1. Add tasks to Tasks sheet (skip first 2 rows)</t>
+    <t xml:space="preserve">  1. Add tasks to TasksTemplates sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">  2. Add templates to TaskTemplates sheet (optional)</t>
+    <t xml:space="preserve">  2. Add employees to Employees sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">  3. Add employees to Employees sheet</t>
+    <t xml:space="preserve">  3. Start adding tasks to the Tasks sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">  4. Upload to HTML app and start tracking!</t>
+    <t xml:space="preserve">  4. Save and Upload to the HTML app and start tracking!</t>
   </si>
   <si>
-    <t>Need help or have suggestions or feedback? find me online : @Mohajiho</t>
+    <t xml:space="preserve">  5. You can also export an Standalone file for your Smart TV</t>
+  </si>
+  <si>
+    <t>Need help or have suggestions or feedback? find me on Twitter/X : @XPRODUCTIVITY</t>
   </si>
 </sst>
 </file>
@@ -408,7 +537,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +636,12 @@
       <color rgb="FFFF5C26"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1083,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1159,67 +1294,57 @@
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20">
-        <v>45986</v>
-      </c>
+      <c r="A5" s="20"/>
       <c r="B5" s="21">
         <v>0.33333333333333331</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="str">
         <f>IF(C5="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C5,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20">
-        <v>45986</v>
-      </c>
+      <c r="A6" s="20"/>
       <c r="B6" s="21">
         <v>0.39583333333333331</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="str">
         <f>IF(C6="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C6,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
-        <v>Entire Store</v>
+        <v/>
       </c>
       <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="20">
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="B7" s="21">
         <v>0.45833333333333331</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="str">
         <f>IF(C7="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C7,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
@@ -1229,11 +1354,9 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="20"/>
@@ -1251,83 +1374,75 @@
       <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="str">
         <f>IF(C9="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C9,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
       <c r="E9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="20">
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="str">
         <f>IF(C10="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C10,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v>Entire Store</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="20">
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="B11" s="21">
         <v>0.91666666666666663</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="str">
         <f>IF(C11="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C11,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
       <c r="E11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="20">
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="str">
         <f>IF(C12="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C12,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
@@ -1339,35 +1454,31 @@
       <c r="F12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="20">
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="str">
         <f>IF(C13="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C13,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v>VMI Only</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B14" s="21">
         <v>0.25</v>
@@ -1385,67 +1496,61 @@
       <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B15" s="21">
         <v>0.33333333333333331</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="str">
         <f>IF(C15="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C15,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
       <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B16" s="21">
         <v>0.41666666666666669</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="str">
         <f>IF(C16="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C16,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v>Entire Store</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B17" s="21">
         <v>0.5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="3" t="str">
         <f>IF(C17="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C17,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
@@ -1457,13 +1562,11 @@
       <c r="F17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="2" t="s">
@@ -1479,38 +1582,36 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="str">
         <f>IF(C19="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C19,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v/>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="20">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D20" s="3" t="str">
         <f>IF(C20="","",IFERROR(INDEX(TaskTemplates!$B$2:$B$1000,MATCH(C20,TaskTemplates!$A$2:$A$1000,0))&amp;"",""))</f>
         <v>Entire Store</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>11</v>
@@ -13363,7 +13464,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>5</v>
@@ -13375,32 +13476,32 @@
         <v>9</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -18407,10 +18508,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18418,12 +18519,12 @@
         <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="10"/>
     </row>
@@ -22426,20 +22527,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A130"/>
+  <dimension ref="A1:A145"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="100" customWidth="1"/>
+    <col min="1" max="1" width="114.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1">
@@ -22447,314 +22548,310 @@
     </row>
     <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="7"/>
+    </row>
+    <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="6"/>
-    </row>
-    <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="8" t="s">
+    <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="6" t="s">
+    <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="23" t="s">
+    <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="6"/>
-    </row>
-    <row r="9" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:1" ht="20.100000000000001" customHeight="1"/>
+    <row r="10" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="8" t="s">
+    <row r="13" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="6"/>
-    </row>
     <row r="16" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1"/>
+    <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="8" t="s">
+    <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="8" t="s">
+    <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="8"/>
-    </row>
-    <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="6"/>
     </row>
     <row r="25" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="8"/>
-    </row>
     <row r="29" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="6"/>
+    </row>
+    <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="32" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>48</v>
+      <c r="A33" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="24" t="s">
-        <v>49</v>
+      <c r="A34" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8"/>
     </row>
     <row r="36" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="24" t="s">
-        <v>50</v>
+      <c r="A36" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="8" t="s">
-        <v>51</v>
+      <c r="A37" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="8" t="s">
-        <v>52</v>
+      <c r="A38" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A39" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="A39" s="6"/>
     </row>
     <row r="40" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="7"/>
+      <c r="A40" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="41" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="25" t="s">
-        <v>54</v>
+      <c r="A41" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="8"/>
+    </row>
+    <row r="44" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="8" t="s">
+    <row r="45" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A45" s="8"/>
-    </row>
     <row r="46" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="24" t="s">
-        <v>58</v>
+      <c r="A46" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A47" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="A47" s="7"/>
     </row>
     <row r="48" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="8"/>
+    </row>
+    <row r="51" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="28" t="s">
+    <row r="52" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A52" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A50" s="6"/>
-    </row>
-    <row r="51" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A51" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="24" t="s">
+    <row r="53" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="8"/>
-    </row>
     <row r="54" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="56" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A56" s="25" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A56" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A59" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A59" s="6"/>
-    </row>
     <row r="60" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="8"/>
+    </row>
+    <row r="61" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A61" s="24" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A61" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A64" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A64" s="7"/>
-    </row>
     <row r="65" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="26" t="s">
-        <v>72</v>
-      </c>
+      <c r="A65" s="6"/>
     </row>
     <row r="66" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="8" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A67" s="8" t="s">
-        <v>74</v>
+      <c r="A67" s="24" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="8"/>
     </row>
     <row r="69" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A69" s="8" t="s">
-        <v>48</v>
+      <c r="A69" s="27" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A70" s="25" t="s">
+      <c r="A70" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A71" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A71" s="8"/>
     </row>
     <row r="72" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="8" t="s">
@@ -22767,246 +22864,317 @@
       </c>
     </row>
     <row r="74" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="6"/>
+    </row>
+    <row r="75" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A75" s="27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A75" s="6" t="s">
+    <row r="76" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A76" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A76" s="23" t="s">
+    <row r="77" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A77" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A77" s="6" t="s">
+    <row r="78" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A78" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A79" s="7"/>
+    </row>
+    <row r="80" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A80" s="26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A79" s="8" t="s">
+    <row r="81" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A81" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A80" s="8" t="s">
+    <row r="82" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A82" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A81" s="8"/>
-    </row>
-    <row r="82" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A82" s="24" t="s">
+    <row r="83" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A83" s="8"/>
+    </row>
+    <row r="84" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A84" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A85" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A83" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A84" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A85" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="86" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A86" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="A86" s="8"/>
     </row>
     <row r="87" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A90" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A91" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A92" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A93" s="8" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A90" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A91" s="6"/>
-    </row>
-    <row r="92" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A92" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A93" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A96" s="8"/>
+    </row>
+    <row r="97" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A97" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A98" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A99" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A96" s="8" t="s">
+    <row r="100" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A100" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
+    <row r="101" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A101" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:1"/>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" ht="15.75">
-      <c r="A100" s="22" t="s">
+    <row r="102" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A102" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:1"/>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
+    <row r="103" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A103" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
+    <row r="104" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A104" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
+    <row r="105" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A105" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
+    <row r="106" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A106" s="6"/>
+    </row>
+    <row r="107" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A107" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1"/>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" ht="15.75">
-      <c r="A108" s="22" t="s">
+    <row r="108" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A108" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:1"/>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
+    <row r="109" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A109" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
+    <row r="110" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A110" s="8" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A111" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
         <v>109</v>
       </c>
     </row>
+    <row r="113" spans="1:1"/>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="15.75">
+      <c r="A115" s="22" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:1"/>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="116" spans="1:1"/>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="118" spans="1:1"/>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:1"/>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="15.75">
+      <c r="A123" s="22" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="s">
-        <v>116</v>
-      </c>
-    </row>
+    <row r="124" spans="1:1"/>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="127" spans="1:1"/>
-    <row r="128" spans="1:1"/>
-    <row r="129" spans="1:1" ht="21">
-      <c r="A129" s="29" t="s">
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
         <v>119</v>
       </c>
     </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="130" spans="1:1"/>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1"/>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1"/>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1"/>
+    <row r="144" spans="1:1" ht="21">
+      <c r="A144" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="145"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="LWO/cjxw+wC0z0l6cSzitWfBo56wDZNC9OKHAVddU0mURnWpF02I5IKHA3E3rc05plbPOuPJaipVorT3JwLmaw==" saltValue="i/hyG32DxJiS60ETH1IHKg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>